<commit_message>
Add quantity list feature
</commit_message>
<xml_diff>
--- a/PharmacyManager/Database.xlsx
+++ b/PharmacyManager/Database.xlsx
@@ -14,57 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>cc2</t>
-  </si>
-  <si>
-    <t>ee2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="5">
   <si>
     <t>Muhammad Zaim Mohamed Pauzi</t>
-  </si>
-  <si>
-    <t>Panadol</t>
-  </si>
-  <si>
-    <t>Ubat 2</t>
-  </si>
-  <si>
-    <t>Ubat 3</t>
-  </si>
-  <si>
-    <t>Ubat 4</t>
-  </si>
-  <si>
-    <t>Ubat 5</t>
-  </si>
-  <si>
-    <t>Ubat 6</t>
-  </si>
-  <si>
-    <t>Ubat 7</t>
-  </si>
-  <si>
-    <t>Ubat 8</t>
-  </si>
-  <si>
-    <t>Ubat 9</t>
-  </si>
-  <si>
-    <t>Ubat 10</t>
-  </si>
-  <si>
-    <t>ff2</t>
   </si>
   <si>
     <t>Abdullah Othman</t>
   </si>
   <si>
-    <t>nameA</t>
+    <t>Name1</t>
   </si>
   <si>
-    <t>nameB</t>
+    <t>Name2</t>
+  </si>
+  <si>
+    <t>Name3</t>
   </si>
 </sst>
 </file>
@@ -409,7 +373,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,37 +387,37 @@
         <v>900826105911</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="J1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="K1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="L1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -461,22 +425,37 @@
         <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>